<commit_message>
Work on Evaluation chapter Some restructuring
</commit_message>
<xml_diff>
--- a/data/Instrument Benchmark Results.xlsx
+++ b/data/Instrument Benchmark Results.xlsx
@@ -191,6 +191,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="0.###&quot;s&quot;" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -231,21 +232,7 @@
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
+                <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
@@ -452,6 +439,7 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:numFmt formatCode="0.###&quot;s&quot;" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -491,21 +479,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
+                <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
@@ -602,11 +576,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1462492032"/>
-        <c:axId val="-1462483328"/>
+        <c:axId val="-766682320"/>
+        <c:axId val="-766674032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1462492032"/>
+        <c:axId val="-766682320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -705,7 +679,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1462483328"/>
+        <c:crossAx val="-766674032"/>
         <c:crossesAt val="0.001"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -713,7 +687,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1462483328"/>
+        <c:axId val="-766674032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -820,7 +794,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1462492032"/>
+        <c:crossAx val="-766682320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -833,7 +807,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1744,7 +1718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E5" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Stick to color scheme, more implementation details.
</commit_message>
<xml_diff>
--- a/data/Instrument Benchmark Results.xlsx
+++ b/data/Instrument Benchmark Results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -145,6 +145,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0C4E6C"/>
+      <color rgb="FFF77200"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -182,7 +188,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="0C4E6C"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -346,7 +352,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="F77200"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -576,11 +582,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-766682320"/>
-        <c:axId val="-766674032"/>
+        <c:axId val="-1508399312"/>
+        <c:axId val="-1481062800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-766682320"/>
+        <c:axId val="-1508399312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +685,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-766674032"/>
+        <c:crossAx val="-1481062800"/>
         <c:crossesAt val="0.001"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -687,7 +693,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-766674032"/>
+        <c:axId val="-1481062800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -794,7 +800,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-766682320"/>
+        <c:crossAx val="-1508399312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>